<commit_message>
must be more tests
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -67,16 +67,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -447,45 +453,57 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1" ht="12.8" customHeight="1" s="2">
-      <c r="A1" s="3" t="inlineStr">
+    <row r="1" ht="12.8" customHeight="1" s="3">
+      <c r="A1" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Content-Type: text/plain; charset="UTF-8"
-Hi It is a test!
+          <t xml:space="preserve">На русском языке
 </t>
         </is>
       </c>
     </row>
-    <row r="2" ht="12.8" customHeight="1" s="2">
-      <c r="A2" s="3" t="inlineStr">
+    <row r="2" ht="12.8" customHeight="1" s="3">
+      <c r="A2" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Content-Type: text/plain; charset="UTF-8"
-Hi! It is a test2
+          <t xml:space="preserve">Вам направлена заявка на комплектацию по номеру заказа № 006863 от
+13.07.2022 15:15:23
+ФИО умершего: Куракина Валентина Степановна
+Дата рождения: 3 декабря 1940 г.
+Дата смерти: 13 июля 2022 г.
+ФИО агента: Воронцов Сергей Георгиевич
+Следующие товары указаны в заказе:
+№
+Артикул
+Содержание
+Количество
+1 7500 Гроб Феникс 1,00
+Комментарий к заказу: Отсутствует
+------------------------------
+--
+Irina Rukavishnikova
+Отправлено из Почты Mail.ru &lt;https://trk.mail.ru/c/zzm979&gt;
 </t>
         </is>
       </c>
     </row>
-    <row r="3" ht="12.8" customHeight="1" s="2">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Content-Type: text/plain; charset="UTF-8"
-Hi!
-It is a test 3
-Go!
-</t>
-        </is>
-      </c>
+    <row r="3" ht="12.8" customHeight="1" s="3">
+      <c r="A3" s="4" t="n"/>
     </row>
-    <row r="5" ht="12.8" customHeight="1" s="2">
-      <c r="A5" s="3" t="n"/>
+    <row r="4" ht="12.8" customHeight="1" s="3">
+      <c r="A4" s="5" t="n"/>
+    </row>
+    <row r="5" ht="12.8" customHeight="1" s="3">
+      <c r="A5" s="4" t="n"/>
+    </row>
+    <row r="6" ht="12.8" customHeight="1" s="3">
+      <c r="A6" s="5" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>